<commit_message>
HtmlUi: - added Ressourcenplanung to Excel
</commit_message>
<xml_diff>
--- a/org.eclipse.scout.rt.ui.html.parent/org.eclipse.scout.rt.ui.html/docs/project_mgmt/Scout Html UI Planung.xlsx
+++ b/org.eclipse.scout.rt.ui.html.parent/org.eclipse.scout.rt.ui.html/docs/project_mgmt/Scout Html UI Planung.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
-    <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
-    <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
+    <sheet name="Aufwand" sheetId="1" r:id="rId1"/>
+    <sheet name="Ressourcen" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="236">
   <si>
     <t>Java Backend</t>
   </si>
@@ -581,9 +580,6 @@
   </si>
   <si>
     <t>noch 30</t>
-  </si>
-  <si>
-    <t>Total Aufwand</t>
   </si>
   <si>
     <t>Erweiterbarkeit</t>
@@ -738,6 +734,48 @@
   </si>
   <si>
     <t>- ViewButton</t>
+  </si>
+  <si>
+    <t>TOTAL Aufwand</t>
+  </si>
+  <si>
+    <t>Html UI %</t>
+  </si>
+  <si>
+    <t>Ferien (Wo.)</t>
+  </si>
+  <si>
+    <t>Html UI PT</t>
+  </si>
+  <si>
+    <t>AWE</t>
+  </si>
+  <si>
+    <t>BSH</t>
+  </si>
+  <si>
+    <t>CGU</t>
+  </si>
+  <si>
+    <t>CRU</t>
+  </si>
+  <si>
+    <t>IMO</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Arbeitstage</t>
+  </si>
+  <si>
+    <t>bis Ende Jahr</t>
+  </si>
+  <si>
+    <t>2015 (prov.)</t>
+  </si>
+  <si>
+    <t>Prognose: Umsetzung gemäss Schätzung (826 PT) Ende 3. Quartal 2015</t>
   </si>
 </sst>
 </file>
@@ -761,7 +799,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -780,8 +818,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -835,11 +891,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -870,6 +937,24 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1314,8 +1399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H166" sqref="H166"/>
+    <sheetView topLeftCell="A139" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A163" sqref="A163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1369,7 +1454,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>173</v>
@@ -1398,7 +1483,7 @@
         <v>64</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8">
@@ -1425,7 +1510,7 @@
         <v>134</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="8">
@@ -1452,7 +1537,7 @@
         <v>136</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8">
@@ -1476,7 +1561,7 @@
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H6" s="9"/>
       <c r="J6" s="8"/>
@@ -1511,7 +1596,7 @@
     </row>
     <row r="8" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B8" s="8">
         <v>8</v>
@@ -1526,7 +1611,7 @@
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H8" s="9"/>
       <c r="J8" s="8"/>
@@ -1536,7 +1621,7 @@
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B9" s="8">
         <v>3</v>
@@ -1551,7 +1636,7 @@
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H9" s="9"/>
       <c r="J9" s="8"/>
@@ -1579,7 +1664,7 @@
         <v>146</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8">
@@ -1967,7 +2052,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="8"/>
@@ -2767,7 +2852,7 @@
         <v>103</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J59" s="8"/>
       <c r="K59" s="8">
@@ -2946,7 +3031,7 @@
         <v>109</v>
       </c>
       <c r="H66" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J66" s="8"/>
       <c r="K66" s="8">
@@ -3088,7 +3173,7 @@
         <v>4</v>
       </c>
       <c r="H73" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J73" s="7"/>
       <c r="K73" s="7"/>
@@ -3113,7 +3198,7 @@
         <v>148</v>
       </c>
       <c r="H74" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J74" s="8"/>
       <c r="K74" s="8">
@@ -3122,7 +3207,7 @@
     </row>
     <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B75" s="8">
         <v>5</v>
@@ -3137,7 +3222,7 @@
       </c>
       <c r="F75" s="8"/>
       <c r="G75" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H75" s="9"/>
       <c r="J75" s="8"/>
@@ -3163,7 +3248,7 @@
         <v>131</v>
       </c>
       <c r="H76" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J76" s="8"/>
       <c r="K76" s="8">
@@ -3187,10 +3272,10 @@
       </c>
       <c r="F77" s="8"/>
       <c r="G77" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H77" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J77" s="8"/>
       <c r="K77" s="8">
@@ -3217,7 +3302,7 @@
         <v>156</v>
       </c>
       <c r="H78" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J78" s="8"/>
       <c r="K78" s="8">
@@ -3251,7 +3336,7 @@
     </row>
     <row r="80" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B80" s="8">
         <v>8</v>
@@ -3266,7 +3351,7 @@
       </c>
       <c r="F80" s="8"/>
       <c r="G80" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H80" s="9"/>
       <c r="J80" s="8"/>
@@ -3291,7 +3376,7 @@
       </c>
       <c r="F81" s="8"/>
       <c r="G81" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H81" s="9"/>
       <c r="J81" s="8">
@@ -3321,7 +3406,7 @@
         <v>147</v>
       </c>
       <c r="H82" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J82" s="8">
         <v>15</v>
@@ -3427,7 +3512,7 @@
       </c>
       <c r="F86" s="8"/>
       <c r="G86" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H86" s="9"/>
       <c r="J86" s="8">
@@ -3439,7 +3524,7 @@
     </row>
     <row r="87" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B87" s="8">
         <v>20</v>
@@ -3454,7 +3539,7 @@
       </c>
       <c r="F87" s="8"/>
       <c r="G87" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H87" s="9"/>
       <c r="J87" s="1"/>
@@ -3479,10 +3564,10 @@
       </c>
       <c r="F88" s="8"/>
       <c r="G88" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H88" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K88" s="8">
         <v>8</v>
@@ -3508,7 +3593,7 @@
         <v>172</v>
       </c>
       <c r="H89" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J89" s="8" t="s">
         <v>175</v>
@@ -3535,7 +3620,7 @@
       <c r="F90" s="8"/>
       <c r="G90" s="9"/>
       <c r="H90" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J90" s="8">
         <v>5</v>
@@ -3970,10 +4055,10 @@
         <v>12.5</v>
       </c>
       <c r="F108" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G108" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H108" s="12"/>
       <c r="J108" s="8" t="s">
@@ -4790,7 +4875,7 @@
       <c r="F140" s="8"/>
       <c r="G140" s="12"/>
       <c r="H140" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J140" s="8">
         <v>15</v>
@@ -4969,7 +5054,7 @@
       <c r="F147" s="8"/>
       <c r="G147" s="12"/>
       <c r="H147" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J147" s="8">
         <v>10</v>
@@ -5030,7 +5115,7 @@
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B150" s="8">
         <v>8</v>
@@ -5098,7 +5183,7 @@
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B154" s="6"/>
       <c r="C154" s="6"/>
@@ -5131,7 +5216,7 @@
         <v>4</v>
       </c>
       <c r="H155" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J155" s="7"/>
       <c r="K155" s="7"/>
@@ -5155,10 +5240,10 @@
       </c>
       <c r="F156" s="8"/>
       <c r="G156" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="H156" s="9" t="s">
         <v>205</v>
-      </c>
-      <c r="H156" s="9" t="s">
-        <v>206</v>
       </c>
       <c r="J156" s="8"/>
       <c r="K156" s="8">
@@ -5167,7 +5252,7 @@
     </row>
     <row r="157" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A157" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B157" s="8">
         <v>30</v>
@@ -5257,7 +5342,7 @@
       </c>
       <c r="F160" s="8"/>
       <c r="G160" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H160" s="9"/>
       <c r="J160" s="8"/>
@@ -5267,7 +5352,7 @@
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B161" s="8">
         <v>5</v>
@@ -5282,10 +5367,10 @@
       </c>
       <c r="F161" s="8"/>
       <c r="G161" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H161" s="9" t="s">
         <v>214</v>
-      </c>
-      <c r="H161" s="9" t="s">
-        <v>215</v>
       </c>
       <c r="J161" s="8" t="s">
         <v>177</v>
@@ -5293,10 +5378,10 @@
       <c r="K161" s="8"/>
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>180</v>
-      </c>
-      <c r="B163">
+      <c r="A163" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="B163" s="22">
         <f>SUM(B3:B160)</f>
         <v>826</v>
       </c>
@@ -5315,7 +5400,7 @@
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B164" s="19">
         <f>E163/B163</f>
@@ -5392,24 +5477,270 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="27">
+        <v>2014</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="23"/>
+      <c r="B2" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="25">
+        <v>80</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3" s="25">
+        <f>$B$10*0.01*B3-(C3*5)</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" s="25">
+        <v>90</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4" s="25">
+        <f t="shared" ref="D4:D7" si="0">$B$10*0.01*B4-(C4*5)</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B5" s="25">
+        <v>85</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" s="25">
+        <f t="shared" si="0"/>
+        <v>102.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B6" s="25">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="25">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B7" s="25">
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" s="25">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="B8" s="29"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="29">
+        <f>SUM(D3:D7)</f>
+        <v>367.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="25"/>
+      <c r="D9" s="25"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B10" s="26">
+        <v>150</v>
+      </c>
+      <c r="C10" t="s">
+        <v>233</v>
+      </c>
+      <c r="D10" s="25"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="23"/>
+      <c r="B13" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>226</v>
+      </c>
+      <c r="B14" s="25">
+        <v>80</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14" s="25">
+        <f>$B$21*0.01*B14-(C14*5)</f>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>227</v>
+      </c>
+      <c r="B15" s="25">
+        <v>90</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15" s="25">
+        <f t="shared" ref="D15:D18" si="1">$B$21*0.01*B15-(C15*5)</f>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B16" s="25">
+        <v>85</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16" s="25">
+        <f t="shared" si="1"/>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>229</v>
+      </c>
+      <c r="B17" s="25">
+        <v>40</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17" s="25">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>230</v>
+      </c>
+      <c r="B18" s="25">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18" s="25">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="29">
+        <f>SUM(D14:D18)</f>
+        <v>654</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="25"/>
+      <c r="D20" s="25"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>232</v>
+      </c>
+      <c r="B21" s="26">
+        <v>240</v>
+      </c>
+      <c r="C21" t="s">
+        <v>233</v>
+      </c>
+      <c r="D21" s="25"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
HtmlUi: Added search outline and some fixes for table selection and session.js
</commit_message>
<xml_diff>
--- a/org.eclipse.scout.rt.ui.html.parent/org.eclipse.scout.rt.ui.html/docs/project_mgmt/Scout Html UI Planung.xlsx
+++ b/org.eclipse.scout.rt.ui.html.parent/org.eclipse.scout.rt.ui.html/docs/project_mgmt/Scout Html UI Planung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Aufwand" sheetId="1" r:id="rId1"/>
@@ -508,10 +508,6 @@
     <t>Request-Optimierung</t>
   </si>
   <si>
-    <t>- Nur an den Server, falls nötig 
-- Prüfung auf method override? Attached Listeners? @gui annotation?</t>
-  </si>
-  <si>
     <t>nur ein tree</t>
   </si>
   <si>
@@ -776,6 +772,11 @@
   </si>
   <si>
     <t>Prognose: Umsetzung gemäss Schätzung (826 PT) Ende 3. Quartal 2015</t>
+  </si>
+  <si>
+    <t>- Nur an den Server, falls nötig 
+- Prüfung auf method override? Attached Listeners? @gui annotation?
+- Nur Daten schicken, die wirklich nötig sind (keine Default-Values)</t>
   </si>
 </sst>
 </file>
@@ -935,8 +936,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -955,6 +954,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1399,8 +1400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M164"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A163" sqref="A163"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1428,10 +1429,10 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="17"/>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="21"/>
+      <c r="K1" s="29"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -1454,13 +1455,13 @@
         <v>4</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J2" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>173</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1483,7 +1484,7 @@
         <v>64</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8">
@@ -1510,7 +1511,7 @@
         <v>134</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="8">
@@ -1537,7 +1538,7 @@
         <v>136</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8">
@@ -1561,7 +1562,7 @@
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H6" s="9"/>
       <c r="J6" s="8"/>
@@ -1596,7 +1597,7 @@
     </row>
     <row r="8" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B8" s="8">
         <v>8</v>
@@ -1611,7 +1612,7 @@
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H8" s="9"/>
       <c r="J8" s="8"/>
@@ -1621,7 +1622,7 @@
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B9" s="8">
         <v>3</v>
@@ -1636,7 +1637,7 @@
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H9" s="9"/>
       <c r="J9" s="8"/>
@@ -1664,7 +1665,7 @@
         <v>146</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8">
@@ -1788,7 +1789,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B17" s="8">
         <v>8</v>
@@ -2028,7 +2029,7 @@
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H26" s="8"/>
       <c r="J26" s="8"/>
@@ -2052,7 +2053,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="8"/>
@@ -2852,7 +2853,7 @@
         <v>103</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J59" s="8"/>
       <c r="K59" s="8">
@@ -3031,7 +3032,7 @@
         <v>109</v>
       </c>
       <c r="H66" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J66" s="8"/>
       <c r="K66" s="8">
@@ -3173,7 +3174,7 @@
         <v>4</v>
       </c>
       <c r="H73" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J73" s="7"/>
       <c r="K73" s="7"/>
@@ -3198,7 +3199,7 @@
         <v>148</v>
       </c>
       <c r="H74" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J74" s="8"/>
       <c r="K74" s="8">
@@ -3207,7 +3208,7 @@
     </row>
     <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B75" s="8">
         <v>5</v>
@@ -3222,7 +3223,7 @@
       </c>
       <c r="F75" s="8"/>
       <c r="G75" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H75" s="9"/>
       <c r="J75" s="8"/>
@@ -3248,7 +3249,7 @@
         <v>131</v>
       </c>
       <c r="H76" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J76" s="8"/>
       <c r="K76" s="8">
@@ -3272,17 +3273,17 @@
       </c>
       <c r="F77" s="8"/>
       <c r="G77" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H77" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J77" s="8"/>
       <c r="K77" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
         <v>155</v>
       </c>
@@ -3299,10 +3300,10 @@
       </c>
       <c r="F78" s="8"/>
       <c r="G78" s="9" t="s">
-        <v>156</v>
+        <v>235</v>
       </c>
       <c r="H78" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J78" s="8"/>
       <c r="K78" s="8">
@@ -3336,7 +3337,7 @@
     </row>
     <row r="80" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B80" s="8">
         <v>8</v>
@@ -3351,7 +3352,7 @@
       </c>
       <c r="F80" s="8"/>
       <c r="G80" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H80" s="9"/>
       <c r="J80" s="8"/>
@@ -3376,7 +3377,7 @@
       </c>
       <c r="F81" s="8"/>
       <c r="G81" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H81" s="9"/>
       <c r="J81" s="8">
@@ -3406,7 +3407,7 @@
         <v>147</v>
       </c>
       <c r="H82" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J82" s="8">
         <v>15</v>
@@ -3512,7 +3513,7 @@
       </c>
       <c r="F86" s="8"/>
       <c r="G86" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H86" s="9"/>
       <c r="J86" s="8">
@@ -3524,7 +3525,7 @@
     </row>
     <row r="87" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B87" s="8">
         <v>20</v>
@@ -3539,7 +3540,7 @@
       </c>
       <c r="F87" s="8"/>
       <c r="G87" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H87" s="9"/>
       <c r="J87" s="1"/>
@@ -3564,10 +3565,10 @@
       </c>
       <c r="F88" s="8"/>
       <c r="G88" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H88" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K88" s="8">
         <v>8</v>
@@ -3575,7 +3576,7 @@
     </row>
     <row r="89" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B89" s="8">
         <v>8</v>
@@ -3590,13 +3591,13 @@
       </c>
       <c r="F89" s="8"/>
       <c r="G89" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H89" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J89" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K89" s="8">
         <v>20</v>
@@ -3604,7 +3605,7 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B90" s="8">
         <v>4</v>
@@ -3620,7 +3621,7 @@
       <c r="F90" s="8"/>
       <c r="G90" s="9"/>
       <c r="H90" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J90" s="8">
         <v>5</v>
@@ -3631,7 +3632,7 @@
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B91" s="8">
         <v>15</v>
@@ -3648,7 +3649,7 @@
       <c r="G91" s="9"/>
       <c r="H91" s="9"/>
       <c r="J91" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K91" s="8">
         <v>15</v>
@@ -3656,7 +3657,7 @@
     </row>
     <row r="92" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B92" s="8">
         <v>5</v>
@@ -3671,11 +3672,11 @@
       </c>
       <c r="F92" s="8"/>
       <c r="G92" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H92" s="9"/>
       <c r="J92" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K92" s="8">
         <v>5</v>
@@ -3727,7 +3728,7 @@
       <c r="G95" s="8"/>
       <c r="H95" s="12"/>
       <c r="J95" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K95" s="8">
         <v>2</v>
@@ -3785,7 +3786,7 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B98" s="8">
         <v>7</v>
@@ -3802,7 +3803,7 @@
       <c r="G98" s="12"/>
       <c r="H98" s="12"/>
       <c r="J98" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K98" s="8">
         <v>7</v>
@@ -3852,7 +3853,7 @@
       <c r="G100" s="12"/>
       <c r="H100" s="12"/>
       <c r="J100" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K100" s="8">
         <v>2</v>
@@ -3877,7 +3878,7 @@
       <c r="G101" s="12"/>
       <c r="H101" s="12"/>
       <c r="J101" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K101" s="8">
         <v>12</v>
@@ -3927,7 +3928,7 @@
       <c r="G103" s="12"/>
       <c r="H103" s="12"/>
       <c r="J103" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K103" s="8">
         <v>2</v>
@@ -3950,11 +3951,11 @@
       </c>
       <c r="F104" s="8"/>
       <c r="G104" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H104" s="12"/>
       <c r="J104" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K104" s="8">
         <v>1</v>
@@ -4029,11 +4030,11 @@
       </c>
       <c r="F107" s="8"/>
       <c r="G107" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H107" s="12"/>
       <c r="J107" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K107" s="8">
         <v>40</v>
@@ -4055,14 +4056,14 @@
         <v>12.5</v>
       </c>
       <c r="F108" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G108" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H108" s="12"/>
       <c r="J108" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K108" s="8">
         <v>15</v>
@@ -4137,7 +4138,7 @@
       <c r="G111" s="12"/>
       <c r="H111" s="12"/>
       <c r="J111" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K111" s="8">
         <v>0</v>
@@ -4159,14 +4160,14 @@
         <v>0</v>
       </c>
       <c r="F112" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G112" s="12" t="s">
         <v>158</v>
-      </c>
-      <c r="G112" s="12" t="s">
-        <v>159</v>
       </c>
       <c r="H112" s="12"/>
       <c r="J112" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K112" s="8">
         <v>0</v>
@@ -4214,11 +4215,11 @@
       </c>
       <c r="F114" s="8"/>
       <c r="G114" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H114" s="12"/>
       <c r="J114" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K114" s="8">
         <v>5</v>
@@ -4266,7 +4267,7 @@
       </c>
       <c r="F116" s="8"/>
       <c r="G116" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H116" s="12"/>
       <c r="J116" s="8">
@@ -4343,7 +4344,7 @@
       </c>
       <c r="F119" s="8"/>
       <c r="G119" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H119" s="12"/>
       <c r="J119" s="8">
@@ -4447,7 +4448,7 @@
       <c r="G123" s="12"/>
       <c r="H123" s="12"/>
       <c r="J123" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K123" s="8">
         <v>5</v>
@@ -4597,7 +4598,7 @@
       <c r="G129" s="12"/>
       <c r="H129" s="12"/>
       <c r="J129" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K129" s="8">
         <v>1</v>
@@ -4622,7 +4623,7 @@
       <c r="G130" s="12"/>
       <c r="H130" s="12"/>
       <c r="J130" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K130" s="8">
         <v>2</v>
@@ -4670,11 +4671,11 @@
       </c>
       <c r="F132" s="8"/>
       <c r="G132" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H132" s="12"/>
       <c r="J132" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K132" s="8">
         <v>2</v>
@@ -4699,7 +4700,7 @@
       <c r="G133" s="12"/>
       <c r="H133" s="12"/>
       <c r="J133" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K133" s="8">
         <v>10</v>
@@ -4749,7 +4750,7 @@
       <c r="G135" s="12"/>
       <c r="H135" s="12"/>
       <c r="J135" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K135" s="8">
         <v>8</v>
@@ -4847,7 +4848,7 @@
       </c>
       <c r="F139" s="8"/>
       <c r="G139" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H139" s="12"/>
       <c r="J139" s="8">
@@ -4875,7 +4876,7 @@
       <c r="F140" s="8"/>
       <c r="G140" s="12"/>
       <c r="H140" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J140" s="8">
         <v>15</v>
@@ -4903,7 +4904,7 @@
       <c r="G141" s="12"/>
       <c r="H141" s="12"/>
       <c r="J141" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K141" s="8">
         <v>2</v>
@@ -5028,7 +5029,7 @@
       <c r="G146" s="12"/>
       <c r="H146" s="12"/>
       <c r="J146" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K146" s="8">
         <v>3</v>
@@ -5054,7 +5055,7 @@
       <c r="F147" s="8"/>
       <c r="G147" s="12"/>
       <c r="H147" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J147" s="8">
         <v>10</v>
@@ -5082,7 +5083,7 @@
       <c r="G148" s="12"/>
       <c r="H148" s="12"/>
       <c r="J148" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K148" s="8">
         <v>2</v>
@@ -5115,7 +5116,7 @@
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B150" s="8">
         <v>8</v>
@@ -5157,7 +5158,7 @@
       <c r="G151" s="12"/>
       <c r="H151" s="12"/>
       <c r="J151" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K151" s="8">
         <v>3</v>
@@ -5183,7 +5184,7 @@
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B154" s="6"/>
       <c r="C154" s="6"/>
@@ -5216,7 +5217,7 @@
         <v>4</v>
       </c>
       <c r="H155" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J155" s="7"/>
       <c r="K155" s="7"/>
@@ -5240,10 +5241,10 @@
       </c>
       <c r="F156" s="8"/>
       <c r="G156" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="H156" s="9" t="s">
         <v>204</v>
-      </c>
-      <c r="H156" s="9" t="s">
-        <v>205</v>
       </c>
       <c r="J156" s="8"/>
       <c r="K156" s="8">
@@ -5252,7 +5253,7 @@
     </row>
     <row r="157" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A157" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B157" s="8">
         <v>30</v>
@@ -5342,7 +5343,7 @@
       </c>
       <c r="F160" s="8"/>
       <c r="G160" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H160" s="9"/>
       <c r="J160" s="8"/>
@@ -5352,7 +5353,7 @@
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B161" s="8">
         <v>5</v>
@@ -5367,21 +5368,21 @@
       </c>
       <c r="F161" s="8"/>
       <c r="G161" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="H161" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="H161" s="9" t="s">
-        <v>214</v>
-      </c>
       <c r="J161" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K161" s="8"/>
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A163" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="B163" s="22">
+      <c r="A163" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="B163" s="20">
         <f>SUM(B3:B160)</f>
         <v>826</v>
       </c>
@@ -5400,7 +5401,7 @@
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B164" s="19">
         <f>E163/B163</f>
@@ -5479,7 +5480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -5492,252 +5493,252 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="27">
+      <c r="A1" s="25">
         <v>2014</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24" t="s">
+      <c r="A2" s="21"/>
+      <c r="B2" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>224</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>226</v>
-      </c>
-      <c r="B3" s="25">
+        <v>225</v>
+      </c>
+      <c r="B3" s="23">
         <v>80</v>
       </c>
       <c r="C3">
         <v>9</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="23">
         <f>$B$10*0.01*B3-(C3*5)</f>
         <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>227</v>
-      </c>
-      <c r="B4" s="25">
+        <v>226</v>
+      </c>
+      <c r="B4" s="23">
         <v>90</v>
       </c>
       <c r="C4">
         <v>6</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="23">
         <f t="shared" ref="D4:D7" si="0">$B$10*0.01*B4-(C4*5)</f>
         <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>228</v>
-      </c>
-      <c r="B5" s="25">
+        <v>227</v>
+      </c>
+      <c r="B5" s="23">
         <v>85</v>
       </c>
       <c r="C5">
         <v>5</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="23">
         <f t="shared" si="0"/>
         <v>102.5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>229</v>
-      </c>
-      <c r="B6" s="25">
+        <v>228</v>
+      </c>
+      <c r="B6" s="23">
         <v>40</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="23">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>230</v>
-      </c>
-      <c r="B7" s="25">
+        <v>229</v>
+      </c>
+      <c r="B7" s="23">
         <v>40</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="23">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="29">
+      <c r="A8" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="27">
         <f>SUM(D3:D7)</f>
         <v>367.5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="25"/>
-      <c r="D9" s="25"/>
+      <c r="B9" s="23"/>
+      <c r="D9" s="23"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>231</v>
+      </c>
+      <c r="B10" s="24">
+        <v>150</v>
+      </c>
+      <c r="C10" t="s">
         <v>232</v>
       </c>
-      <c r="B10" s="26">
-        <v>150</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" s="23"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
         <v>233</v>
       </c>
-      <c r="D10" s="25"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
-        <v>234</v>
-      </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="24" t="s">
+      <c r="A13" s="21"/>
+      <c r="B13" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="C13" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="D13" s="22" t="s">
         <v>224</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>226</v>
-      </c>
-      <c r="B14" s="25">
+        <v>225</v>
+      </c>
+      <c r="B14" s="23">
         <v>80</v>
       </c>
       <c r="C14">
         <v>6</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="23">
         <f>$B$21*0.01*B14-(C14*5)</f>
         <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>227</v>
-      </c>
-      <c r="B15" s="25">
+        <v>226</v>
+      </c>
+      <c r="B15" s="23">
         <v>90</v>
       </c>
       <c r="C15">
         <v>6</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15" s="23">
         <f t="shared" ref="D15:D18" si="1">$B$21*0.01*B15-(C15*5)</f>
         <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>228</v>
-      </c>
-      <c r="B16" s="25">
+        <v>227</v>
+      </c>
+      <c r="B16" s="23">
         <v>85</v>
       </c>
       <c r="C16">
         <v>6</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="23">
         <f t="shared" si="1"/>
         <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>229</v>
-      </c>
-      <c r="B17" s="25">
+        <v>228</v>
+      </c>
+      <c r="B17" s="23">
         <v>40</v>
       </c>
       <c r="C17">
         <v>6</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="23">
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>230</v>
-      </c>
-      <c r="B18" s="25">
+        <v>229</v>
+      </c>
+      <c r="B18" s="23">
         <v>40</v>
       </c>
       <c r="C18">
         <v>6</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="23">
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="29">
+      <c r="A19" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="27">
         <f>SUM(D14:D18)</f>
         <v>654</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="25"/>
-      <c r="D20" s="25"/>
+      <c r="B20" s="23"/>
+      <c r="D20" s="23"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>231</v>
+      </c>
+      <c r="B21" s="24">
+        <v>240</v>
+      </c>
+      <c r="C21" t="s">
         <v>232</v>
       </c>
-      <c r="B21" s="26">
-        <v>240</v>
-      </c>
-      <c r="C21" t="s">
-        <v>233</v>
-      </c>
-      <c r="D21" s="25"/>
+      <c r="D21" s="23"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
-        <v>235</v>
+      <c r="A23" s="20" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>